<commit_message>
Updated all test xlsx files to use MNRF rather than OMNR
</commit_message>
<xml_diff>
--- a/fsdviz/tests/xls_files/missing_one_field.xlsx
+++ b/fsdviz/tests/xls_files/missing_one_field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COTTRILLAD\1work\LakeTrout\Stocking\GLFSD_Datavis\fsdviz\fsdviz\tests\xls_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1work\fsdviz\fsdviz\tests\xls_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21AAE0A-6FA8-44D0-A289-315A4585A711}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4650DD7-BB36-4C26-80E5-DED6E93C8F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B75592B0-B996-4C91-8D85-EEB976D88E37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B75592B0-B996-4C91-8D85-EEB976D88E37}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_TEMPLATE" sheetId="2" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Enter\paste your data below:</t>
   </si>
   <si>
-    <t>OMNR</t>
-  </si>
-  <si>
     <t>HU</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>Chatsworth</t>
+  </si>
+  <si>
+    <t>MNRF</t>
   </si>
 </sst>
 </file>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4BD917-88B4-41AD-94D6-751B8B921A3A}">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1338,26 +1338,26 @@
         <v>42701</v>
       </c>
       <c r="C10" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="E10" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="F10" s="57" t="s">
         <v>56</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>57</v>
       </c>
       <c r="G10" s="57"/>
       <c r="H10" s="56">
         <v>1128</v>
       </c>
       <c r="I10" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="57" t="s">
         <v>58</v>
-      </c>
-      <c r="J10" s="57" t="s">
-        <v>59</v>
       </c>
       <c r="K10" s="56">
         <v>44.566400000000002</v>
@@ -1381,7 +1381,7 @@
         <v>46</v>
       </c>
       <c r="R10" s="57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S10" s="57" t="s">
         <v>48</v>
@@ -1390,7 +1390,7 @@
         <v>16</v>
       </c>
       <c r="U10" s="57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V10" s="58"/>
       <c r="W10" s="57"/>
@@ -1408,7 +1408,7 @@
         <v>380</v>
       </c>
       <c r="AE10" s="57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF10" s="56">
         <v>30747</v>

</xml_diff>